<commit_message>
Adding data into show products by brands
</commit_message>
<xml_diff>
--- a/StaticSite/assets/ProductsInfo.xlsx
+++ b/StaticSite/assets/ProductsInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\1512012_1512013\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\Web\FinalProject\1512012_1512013_PTUDW\StaticSite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B143822-E699-4024-865C-9D9A7A341F38}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC278C3-488A-4242-ADA4-8981286F97C6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{7FC2539B-84A1-45CB-BC2F-CF565FDC9752}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
-  <si>
-    <t>Máy Ảnh Canon EOS 3000D + Lens EF-S 18 - 55mm III (Lê Bảo Minh)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="102">
   <si>
     <t>Máy Ảnh Canon EOS M50 + Kit 15-45mm (24.1MP) (Lê Bảo Minh)</t>
   </si>
@@ -1008,7 +1005,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1027,89 +1024,89 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1">
         <v>6</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1">
         <v>7</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1120,13 +1117,13 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -1135,13 +1132,13 @@
     <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1">
         <v>4</v>
@@ -1150,13 +1147,13 @@
     <row r="8" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A8" s="23"/>
       <c r="B8" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="D8" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="1">
         <v>8</v>
@@ -1165,13 +1162,13 @@
     <row r="9" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>80</v>
-      </c>
       <c r="D9" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="1">
         <v>9</v>
@@ -1180,13 +1177,13 @@
     <row r="10" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>78</v>
-      </c>
       <c r="D10" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
@@ -1195,13 +1192,13 @@
     <row r="11" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="D11" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="1">
         <v>11</v>
@@ -1210,13 +1207,13 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1">
         <v>5</v>
@@ -1230,88 +1227,88 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="D14" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="D15" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="D16" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A18" s="24"/>
       <c r="B18" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>99</v>
-      </c>
       <c r="D18" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
       <c r="B19" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>101</v>
-      </c>
       <c r="D19" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1322,244 +1319,244 @@
     </row>
     <row r="22" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>16</v>
-      </c>
       <c r="D22" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A23" s="30"/>
       <c r="B23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="D23" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
       <c r="B24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="D24" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A25" s="30"/>
       <c r="B25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="D25" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
       <c r="B26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="D26" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="30"/>
       <c r="B27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="D27" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="D28" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A29" s="30"/>
       <c r="B29" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
       <c r="B30" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="D30" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A32" s="30"/>
       <c r="B32" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>68</v>
-      </c>
       <c r="D32" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A33" s="30"/>
       <c r="B33" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>84</v>
-      </c>
       <c r="D33" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A34" s="30"/>
       <c r="B34" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>86</v>
-      </c>
       <c r="D34" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A35" s="30"/>
       <c r="B35" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>88</v>
-      </c>
       <c r="D35" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A36" s="30"/>
       <c r="B36" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>90</v>
-      </c>
       <c r="D36" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A37" s="30"/>
       <c r="B37" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A38" s="30"/>
       <c r="B38" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="D38" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
       <c r="B39" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>97</v>
-      </c>
       <c r="D39" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A40" s="30"/>
       <c r="B40" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>95</v>
-      </c>
       <c r="D40" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A41" s="31"/>
       <c r="B41" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,100 +1567,100 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
       <c r="B44" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="D44" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="D45" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="25"/>
       <c r="B47" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C48" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="D48" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="25"/>
       <c r="B49" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="D49" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
       <c r="B50" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="D50" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>